<commit_message>
fix counterparties / transaction attributes
</commit_message>
<xml_diff>
--- a/resources/obp-data-import_template.xlsx
+++ b/resources/obp-data-import_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Banks" sheetId="1" state="visible" r:id="rId2"/>
@@ -181,7 +181,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -202,11 +202,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -263,7 +258,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,14 +267,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,7 +291,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,10 +379,10 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="Q:Q F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
@@ -432,27 +435,27 @@
   </sheetPr>
   <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P1" activeCellId="1" sqref="Q:Q P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="22.51"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="17.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="22.51"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="5" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="5" width="17.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="5" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="19.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="21.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="4" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="22.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="6" width="21.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.45"/>
   </cols>
@@ -464,34 +467,34 @@
       <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="0" t="s">
@@ -500,7 +503,7 @@
       <c r="N1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>20</v>
       </c>
       <c r="P1" s="6" t="s">
@@ -528,13 +531,13 @@
   </sheetPr>
   <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q:Q"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.1"/>
@@ -547,12 +550,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="28.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="10"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="16" style="4" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="16" style="9" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -597,10 +600,10 @@
       <c r="O1" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="9" t="s">
         <v>38</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -626,16 +629,16 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="1" sqref="Q:Q C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="16.02"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="19.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="19.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="19.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.39"/>
   </cols>
@@ -650,10 +653,10 @@
       <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>43</v>
       </c>
       <c r="F1" s="1" t="s">

</xml_diff>